<commit_message>
Updated site changes 4/22
</commit_message>
<xml_diff>
--- a/products.xlsx
+++ b/products.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10123"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21929"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Library/WebServer/Documents/cs360_project1-master/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\14794\Desktop\projects\cs360_project1-master\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7CE453A9-538B-4345-A8F5-4C5F1F3B6AC9}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{67C89D88-AFC5-4B50-8935-3EEB0BDB3EC1}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="760" yWindow="480" windowWidth="28040" windowHeight="16500" xr2:uid="{4A75A725-0A3C-E54C-A6C1-2BCFBC86A870}"/>
+    <workbookView xWindow="-19410" yWindow="5895" windowWidth="26505" windowHeight="11400" xr2:uid="{4A75A725-0A3C-E54C-A6C1-2BCFBC86A870}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -30,52 +30,38 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
-  <si>
-    <t xml:space="preserve">Name </t>
-  </si>
-  <si>
-    <t>Description</t>
-  </si>
-  <si>
-    <t>Image</t>
-  </si>
-  <si>
-    <t>Price</t>
-  </si>
-  <si>
-    <t>This is the discription of the first product. It was develeoped by me when I was bored. Blah Blah Whats up?</t>
-  </si>
-  <si>
-    <t>This is the discription of the second product. It was develeoped by me when I was bored. Blah Blah Whats up?</t>
-  </si>
-  <si>
-    <t>Iphone 3GS</t>
-  </si>
-  <si>
-    <t>img/Logo.png</t>
-  </si>
-  <si>
-    <t>Iphone 4GS</t>
-  </si>
-  <si>
-    <t>img/profile_placeholder.jpg</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="8">
+  <si>
+    <t>EndStrips</t>
+  </si>
+  <si>
+    <t>EndCaps</t>
+  </si>
+  <si>
+    <t>Extended release glucose capsules. Never worry about hypoglycemia at night again!</t>
+  </si>
+  <si>
+    <t>img/endcaps.png</t>
+  </si>
+  <si>
+    <t>Revolutionary micro-dosing hypoglycemic system. Developed in house by EndT1.</t>
+  </si>
+  <si>
+    <t>img/endstrips.png</t>
+  </si>
+  <si>
+    <t>test</t>
+  </si>
+  <si>
+    <t>asdfasd</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
-      <sz val="12"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
       <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -105,7 +91,7 @@
   </cellStyleXfs>
   <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -423,57 +409,57 @@
   <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="18.5" customWidth="1"/>
-    <col min="2" max="2" width="61" customWidth="1"/>
-    <col min="3" max="3" width="17.33203125" customWidth="1"/>
-    <col min="4" max="4" width="26.1640625" customWidth="1"/>
+    <col min="1" max="1" width="8.375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="71" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="5.375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="26.125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1" s="1">
+        <v>10</v>
+      </c>
+      <c r="D1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="B2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" s="1">
+        <v>10</v>
+      </c>
+      <c r="D2" t="s">
         <v>3</v>
       </c>
-      <c r="D1" s="1" t="s">
-        <v>2</v>
-      </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
-        <v>8</v>
-      </c>
-      <c r="B2" t="s">
-        <v>4</v>
-      </c>
-      <c r="C2">
-        <v>20.100000000000001</v>
-      </c>
-      <c r="D2" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>6</v>
       </c>
       <c r="B3" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="C3">
-        <v>30.56</v>
+        <v>12</v>
       </c>
       <c r="D3" t="s">
-        <v>9</v>
+        <v>3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>